<commit_message>
allow quantifer instead `is_quantifer` for backwards compatibility
</commit_message>
<xml_diff>
--- a/inst/extdata/S1P_metadata_tables.xlsx
+++ b/inst/extdata/S1P_metadata_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6027616-53B4-5144-98A8-622716AE0AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7433C8-43B0-0E47-8E60-69A12643252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9580" yWindow="12600" windowWidth="42840" windowHeight="17440" activeTab="1" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
@@ -3794,7 +3794,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:J17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>